<commit_message>
Updated Gantt Chart with new tasks from 1-11-12 meeting
</commit_message>
<xml_diff>
--- a/n15/docs/Gantt-chart.xlsx
+++ b/n15/docs/Gantt-chart.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="76" count="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="78" count="99">
   <si>
     <t>ID</t>
   </si>
@@ -142,13 +142,19 @@
     <t>Detailed Design</t>
   </si>
   <si>
+    <t>SE_N15_DS_06</t>
+  </si>
+  <si>
+    <t>Kamil Mrowic</t>
+  </si>
+  <si>
+    <t>Researching DBMS Systems (Prosgres vs MySql)</t>
+  </si>
+  <si>
     <t>SE_N15_CODE_01</t>
   </si>
   <si>
     <t>CODE_02 - 04</t>
-  </si>
-  <si>
-    <t>Kamil Mrowic</t>
   </si>
   <si>
     <t>Prototypes</t>
@@ -430,7 +436,7 @@
         <v>41210</v>
       </c>
       <c s="1" r="E7">
-        <v>41229</v>
+        <v>41223</v>
       </c>
       <c t="s" r="F7">
         <v>24</v>
@@ -574,28 +580,28 @@
       <c t="s" r="A15">
         <v>43</v>
       </c>
-      <c t="s" r="B15">
+      <c t="s" r="C15">
         <v>44</v>
       </c>
-      <c t="s" r="C15">
+      <c s="1" r="D15">
+        <v>41214</v>
+      </c>
+      <c s="1" r="E15">
+        <v>41221</v>
+      </c>
+      <c t="s" r="F15">
         <v>45</v>
-      </c>
-      <c s="1" r="D15">
-        <v>41215</v>
-      </c>
-      <c s="1" r="E15">
-        <v>41244</v>
-      </c>
-      <c t="s" r="F15">
-        <v>46</v>
       </c>
     </row>
     <row r="16">
       <c t="s" r="A16">
+        <v>46</v>
+      </c>
+      <c t="s" r="B16">
         <v>47</v>
       </c>
       <c t="s" r="C16">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c s="1" r="D16">
         <v>41215</v>
@@ -612,10 +618,10 @@
         <v>49</v>
       </c>
       <c t="s" r="C17">
-        <v>15</v>
+        <v>44</v>
       </c>
       <c s="1" r="D17">
-        <v>41230</v>
+        <v>41215</v>
       </c>
       <c s="1" r="E17">
         <v>41244</v>
@@ -629,10 +635,10 @@
         <v>51</v>
       </c>
       <c t="s" r="C18">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c s="1" r="D18">
-        <v>41215</v>
+        <v>41230</v>
       </c>
       <c s="1" r="E18">
         <v>41244</v>
@@ -645,39 +651,39 @@
       <c t="s" r="A19">
         <v>53</v>
       </c>
-      <c t="s" r="B19">
+      <c t="s" r="C19">
+        <v>9</v>
+      </c>
+      <c s="1" r="D19">
+        <v>41215</v>
+      </c>
+      <c s="1" r="E19">
+        <v>41244</v>
+      </c>
+      <c t="s" r="F19">
         <v>54</v>
-      </c>
-      <c t="s" r="C19">
-        <v>45</v>
-      </c>
-      <c s="1" r="D19">
-        <v>41244</v>
-      </c>
-      <c s="1" r="E19">
-        <v>41310</v>
-      </c>
-      <c t="s" r="F19">
-        <v>55</v>
-      </c>
-      <c t="s" r="G19">
-        <v>56</v>
       </c>
     </row>
     <row r="20">
       <c t="s" r="A20">
+        <v>55</v>
+      </c>
+      <c t="s" r="B20">
+        <v>56</v>
+      </c>
+      <c t="s" r="C20">
+        <v>44</v>
+      </c>
+      <c s="1" r="D20">
+        <v>41244</v>
+      </c>
+      <c s="1" r="E20">
+        <v>41310</v>
+      </c>
+      <c t="s" r="F20">
         <v>57</v>
       </c>
-      <c t="s" r="C20">
-        <v>41</v>
-      </c>
-      <c s="1" r="D20">
-        <v>41303</v>
-      </c>
-      <c s="1" r="E20">
-        <v>41315</v>
-      </c>
-      <c t="s" r="F20">
+      <c t="s" r="G20">
         <v>58</v>
       </c>
     </row>
@@ -686,7 +692,7 @@
         <v>59</v>
       </c>
       <c t="s" r="C21">
-        <v>28</v>
+        <v>41</v>
       </c>
       <c s="1" r="D21">
         <v>41303</v>
@@ -703,30 +709,24 @@
         <v>61</v>
       </c>
       <c t="s" r="C22">
-        <v>9</v>
+        <v>28</v>
       </c>
       <c s="1" r="D22">
-        <v>40945</v>
+        <v>41303</v>
       </c>
       <c s="1" r="E22">
-        <v>40955</v>
+        <v>41315</v>
       </c>
       <c t="s" r="F22">
         <v>62</v>
       </c>
-      <c t="s" r="G22">
-        <v>63</v>
-      </c>
     </row>
     <row r="23">
       <c t="s" r="A23">
-        <v>64</v>
-      </c>
-      <c t="s" r="B23">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c t="s" r="C23">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c s="1" r="D23">
         <v>40945</v>
@@ -735,18 +735,21 @@
         <v>40955</v>
       </c>
       <c t="s" r="F23">
-        <v>66</v>
+        <v>64</v>
+      </c>
+      <c t="s" r="G23">
+        <v>65</v>
       </c>
     </row>
     <row r="24">
       <c t="s" r="A24">
+        <v>66</v>
+      </c>
+      <c t="s" r="B24">
         <v>67</v>
       </c>
-      <c t="s" r="B24">
-        <v>68</v>
-      </c>
       <c t="s" r="C24">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c s="1" r="D24">
         <v>40945</v>
@@ -755,38 +758,38 @@
         <v>40955</v>
       </c>
       <c t="s" r="F24">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="25">
       <c t="s" r="A25">
+        <v>69</v>
+      </c>
+      <c t="s" r="B25">
         <v>70</v>
       </c>
-      <c t="s" r="B25">
-        <v>71</v>
-      </c>
       <c t="s" r="C25">
-        <v>41</v>
+        <v>23</v>
       </c>
       <c s="1" r="D25">
-        <v>40949</v>
+        <v>40945</v>
       </c>
       <c s="1" r="E25">
         <v>40955</v>
       </c>
       <c t="s" r="F25">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="26">
       <c t="s" r="A26">
+        <v>72</v>
+      </c>
+      <c t="s" r="B26">
         <v>73</v>
       </c>
-      <c t="s" r="B26">
-        <v>74</v>
-      </c>
       <c t="s" r="C26">
-        <v>28</v>
+        <v>41</v>
       </c>
       <c s="1" r="D26">
         <v>40949</v>
@@ -795,7 +798,27 @@
         <v>40955</v>
       </c>
       <c t="s" r="F26">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="27">
+      <c t="s" r="A27">
         <v>75</v>
+      </c>
+      <c t="s" r="B27">
+        <v>76</v>
+      </c>
+      <c t="s" r="C27">
+        <v>28</v>
+      </c>
+      <c s="1" r="D27">
+        <v>40949</v>
+      </c>
+      <c s="1" r="E27">
+        <v>40955</v>
+      </c>
+      <c t="s" r="F27">
+        <v>77</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Misspelled name on Gantt-chart corrected.
</commit_message>
<xml_diff>
--- a/n15/docs/Gantt-chart.xlsx
+++ b/n15/docs/Gantt-chart.xlsx
@@ -1,17 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="Calc"/>
+  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
+  <workbookProtection/>
+  <bookViews>
+    <workbookView activeTab="0" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="600" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
+  </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="78" count="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="78">
   <si>
     <t>ID</t>
   </si>
@@ -145,7 +149,7 @@
     <t>SE_N15_DS_06</t>
   </si>
   <si>
-    <t>Kamil Mrowic</t>
+    <t>Kamil Mrowiec</t>
   </si>
   <si>
     <t>Researching DBMS Systems (Prosgres vs MySql)</t>
@@ -250,19 +254,33 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="m/d/yyyy;@"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="2">
+    <numFmt formatCode="GENERAL" numFmtId="164"/>
+    <numFmt formatCode="M/D/YYYY;@" numFmtId="165"/>
   </numFmts>
-  <fonts count="1">
+  <fonts count="4">
     <font>
-      <b val="0"/>
-      <i val="0"/>
-      <strike val="0"/>
-      <u val="none"/>
-      <sz val="10.0"/>
-      <color rgb="FF000000"/>
       <name val="Arial"/>
+      <charset val="1"/>
+      <family val="2"/>
+      <color rgb="00000000"/>
+      <sz val="10"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <family val="0"/>
+      <sz val="10"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <family val="0"/>
+      <sz val="10"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <family val="0"/>
+      <sz val="10"/>
     </font>
   </fonts>
   <fills count="2">
@@ -270,13 +288,11 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="gray125">
-        <bgColor rgb="FFFFFFFF"/>
-      </patternFill>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
   <borders count="1">
-    <border>
+    <border diagonalDown="false" diagonalUp="false">
       <left/>
       <right/>
       <top/>
@@ -284,543 +300,582 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+  <cellStyleXfs count="20">
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="0" numFmtId="164">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="43"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="41"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="44"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="42"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="9"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="0" xfId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1">
-      <alignment horizontal="general" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" xfId="0" applyNumberFormat="1" fontId="0" fillId="0" borderId="0" applyAlignment="1">
-      <alignment horizontal="general" vertical="bottom" wrapText="1"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
+    <xf applyAlignment="true" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="165" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="true"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+  <cellStyles count="6">
+    <cellStyle builtinId="0" customBuiltin="false" name="Normal" xfId="0"/>
+    <cellStyle builtinId="3" customBuiltin="false" name="Comma" xfId="15"/>
+    <cellStyle builtinId="6" customBuiltin="false" name="Comma [0]" xfId="16"/>
+    <cellStyle builtinId="4" customBuiltin="false" name="Currency" xfId="17"/>
+    <cellStyle builtinId="7" customBuiltin="false" name="Currency [0]" xfId="18"/>
+    <cellStyle builtinId="5" customBuiltin="false" name="Percent" xfId="19"/>
   </cellStyles>
 </styleSheet>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:G27"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="G13" activeCellId="0" pane="topLeft" sqref="G13"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" defaultColWidth="17.14" customHeight="1"/>
   <cols>
-    <col max="1" min="1" customWidth="1" width="20.71"/>
-    <col max="2" min="2" customWidth="1" width="27.86"/>
-    <col max="6" min="6" customWidth="1" width="42.14"/>
-    <col max="7" min="7" customWidth="1" width="37.14"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.8117647058824"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="28"/>
+    <col collapsed="false" hidden="false" max="5" min="3" style="0" width="17.2196078431373"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="42.3450980392157"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="37.3254901960784"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="17.2196078431373"/>
   </cols>
   <sheetData>
-    <row r="1">
-      <c t="s" r="A1">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="1">
+      <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
-      <c t="s" r="B1">
+      <c r="B1" s="0" t="s">
         <v>1</v>
       </c>
-      <c t="s" r="C1">
+      <c r="C1" s="0" t="s">
         <v>2</v>
       </c>
-      <c t="s" r="D1">
+      <c r="D1" s="0" t="s">
         <v>3</v>
       </c>
-      <c t="s" r="E1">
+      <c r="E1" s="0" t="s">
         <v>4</v>
       </c>
-      <c t="s" r="F1">
+      <c r="F1" s="0" t="s">
         <v>5</v>
       </c>
-      <c t="s" r="G1">
+      <c r="G1" s="0" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2">
-      <c t="s" r="A2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="2">
+      <c r="A2" s="0" t="s">
         <v>7</v>
       </c>
-      <c t="s" r="B2">
+      <c r="B2" s="0" t="s">
         <v>8</v>
       </c>
-      <c t="s" r="C2">
+      <c r="C2" s="0" t="s">
         <v>9</v>
       </c>
-      <c s="1" r="D2">
+      <c r="D2" s="1" t="n">
         <v>41191</v>
       </c>
-      <c s="1" r="E2">
+      <c r="E2" s="1" t="n">
         <v>41214</v>
       </c>
-      <c t="s" r="F2">
+      <c r="F2" s="0" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="3">
-      <c t="s" r="A3">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="3">
+      <c r="A3" s="0" t="s">
         <v>11</v>
       </c>
-      <c t="s" r="C3">
+      <c r="C3" s="0" t="s">
         <v>12</v>
       </c>
-      <c s="1" r="D3">
+      <c r="D3" s="1" t="n">
         <v>41191</v>
       </c>
-      <c s="1" r="E3">
+      <c r="E3" s="1" t="n">
         <v>41214</v>
       </c>
-      <c t="s" r="F3">
+      <c r="F3" s="0" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="4">
-      <c t="s" r="A4">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="4">
+      <c r="A4" s="0" t="s">
         <v>14</v>
       </c>
-      <c t="s" r="C4">
+      <c r="C4" s="0" t="s">
         <v>15</v>
       </c>
-      <c s="1" r="D4">
+      <c r="D4" s="1" t="n">
         <v>41191</v>
       </c>
-      <c s="1" r="E4">
+      <c r="E4" s="1" t="n">
         <v>41214</v>
       </c>
-      <c t="s" r="F4">
+      <c r="F4" s="0" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="5">
-      <c t="s" r="A5">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="5">
+      <c r="A5" s="0" t="s">
         <v>17</v>
       </c>
-      <c t="s" r="C5">
+      <c r="C5" s="0" t="s">
         <v>18</v>
       </c>
-      <c s="1" r="D5">
+      <c r="D5" s="1" t="n">
         <v>41191</v>
       </c>
-      <c s="1" r="E5">
+      <c r="E5" s="1" t="n">
         <v>41214</v>
       </c>
-      <c t="s" r="F5">
+      <c r="F5" s="0" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="6">
-      <c t="s" r="A6">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="6">
+      <c r="A6" s="0" t="s">
         <v>20</v>
       </c>
-      <c t="s" r="C6">
+      <c r="C6" s="0" t="s">
         <v>9</v>
       </c>
-      <c s="1" r="D6">
+      <c r="D6" s="1" t="n">
         <v>41191</v>
       </c>
-      <c s="1" r="E6">
+      <c r="E6" s="1" t="n">
         <v>41214</v>
       </c>
-      <c t="s" r="F6">
+      <c r="F6" s="0" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="7">
-      <c t="s" r="A7">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="7">
+      <c r="A7" s="0" t="s">
         <v>22</v>
       </c>
-      <c t="s" r="C7">
+      <c r="C7" s="0" t="s">
         <v>23</v>
       </c>
-      <c s="1" r="D7">
+      <c r="D7" s="1" t="n">
         <v>41210</v>
       </c>
-      <c s="1" r="E7">
+      <c r="E7" s="1" t="n">
         <v>41223</v>
       </c>
-      <c t="s" r="F7">
+      <c r="F7" s="0" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="8">
-      <c t="s" r="A8">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="8">
+      <c r="A8" s="0" t="s">
         <v>25</v>
       </c>
-      <c t="s" r="B8">
+      <c r="B8" s="0" t="s">
         <v>26</v>
       </c>
-      <c t="s" r="C8">
+      <c r="C8" s="0" t="s">
         <v>23</v>
       </c>
-      <c s="1" r="D8">
+      <c r="D8" s="1" t="n">
         <v>41244</v>
       </c>
-      <c s="1" r="E8">
+      <c r="E8" s="1" t="n">
         <v>41282</v>
       </c>
-      <c t="s" r="F8">
+      <c r="F8" s="0" t="s">
         <v>27</v>
       </c>
-      <c t="s" r="G8">
+      <c r="G8" s="0" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="9">
-      <c t="s" r="A9">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="9">
+      <c r="A9" s="0" t="s">
         <v>29</v>
       </c>
-      <c t="s" r="B9">
+      <c r="B9" s="0" t="s">
         <v>30</v>
       </c>
-      <c t="s" r="C9">
+      <c r="C9" s="0" t="s">
         <v>23</v>
       </c>
-      <c s="1" r="D9">
+      <c r="D9" s="1" t="n">
         <v>40937</v>
       </c>
-      <c s="1" r="E9">
+      <c r="E9" s="1" t="n">
         <v>41309</v>
       </c>
-      <c t="s" r="F9">
+      <c r="F9" s="0" t="s">
         <v>31</v>
       </c>
-      <c t="s" r="G9">
+      <c r="G9" s="0" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="10">
-      <c t="s" r="A10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="10">
+      <c r="A10" s="0" t="s">
         <v>32</v>
       </c>
-      <c t="s" r="B10">
+      <c r="B10" s="0" t="s">
         <v>33</v>
       </c>
-      <c t="s" r="C10">
+      <c r="C10" s="0" t="s">
         <v>18</v>
       </c>
-      <c s="1" r="D10">
+      <c r="D10" s="1" t="n">
         <v>41215</v>
       </c>
-      <c s="1" r="E10">
+      <c r="E10" s="1" t="n">
         <v>41254</v>
       </c>
-      <c t="s" r="F10">
+      <c r="F10" s="0" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="11">
-      <c t="s" r="A11">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="11">
+      <c r="A11" s="0" t="s">
         <v>34</v>
       </c>
-      <c t="s" r="C11">
+      <c r="C11" s="0" t="s">
         <v>28</v>
       </c>
-      <c s="1" r="D11">
+      <c r="D11" s="1" t="n">
         <v>41215</v>
       </c>
-      <c s="1" r="E11">
+      <c r="E11" s="1" t="n">
         <v>41229</v>
       </c>
-      <c t="s" r="F11">
+      <c r="F11" s="0" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="12">
-      <c t="s" r="A12">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="12">
+      <c r="A12" s="0" t="s">
         <v>36</v>
       </c>
-      <c t="s" r="C12">
+      <c r="C12" s="0" t="s">
         <v>15</v>
       </c>
-      <c s="1" r="D12">
+      <c r="D12" s="1" t="n">
         <v>41215</v>
       </c>
-      <c s="1" r="E12">
+      <c r="E12" s="1" t="n">
         <v>41229</v>
       </c>
-      <c t="s" r="F12">
+      <c r="F12" s="0" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="13">
-      <c t="s" r="A13">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="13">
+      <c r="A13" s="0" t="s">
         <v>38</v>
       </c>
-      <c t="s" r="C13">
+      <c r="C13" s="0" t="s">
         <v>12</v>
       </c>
-      <c s="1" r="D13">
+      <c r="D13" s="1" t="n">
         <v>41215</v>
       </c>
-      <c s="1" r="E13">
+      <c r="E13" s="1" t="n">
         <v>41229</v>
       </c>
-      <c t="s" r="F13">
+      <c r="F13" s="0" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="14">
-      <c t="s" r="A14">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="14">
+      <c r="A14" s="0" t="s">
         <v>40</v>
       </c>
-      <c t="s" r="C14">
+      <c r="C14" s="0" t="s">
         <v>41</v>
       </c>
-      <c s="1" r="D14">
+      <c r="D14" s="1" t="n">
         <v>41215</v>
       </c>
-      <c s="1" r="E14">
+      <c r="E14" s="1" t="n">
         <v>41229</v>
       </c>
-      <c t="s" r="F14">
+      <c r="F14" s="0" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="15">
-      <c t="s" r="A15">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="15">
+      <c r="A15" s="0" t="s">
         <v>43</v>
       </c>
-      <c t="s" r="C15">
+      <c r="C15" s="0" t="s">
         <v>44</v>
       </c>
-      <c s="1" r="D15">
+      <c r="D15" s="1" t="n">
         <v>41214</v>
       </c>
-      <c s="1" r="E15">
+      <c r="E15" s="1" t="n">
         <v>41221</v>
       </c>
-      <c t="s" r="F15">
+      <c r="F15" s="0" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="16">
-      <c t="s" r="A16">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="16">
+      <c r="A16" s="0" t="s">
         <v>46</v>
       </c>
-      <c t="s" r="B16">
+      <c r="B16" s="0" t="s">
         <v>47</v>
       </c>
-      <c t="s" r="C16">
+      <c r="C16" s="0" t="s">
         <v>44</v>
       </c>
-      <c s="1" r="D16">
+      <c r="D16" s="1" t="n">
         <v>41215</v>
       </c>
-      <c s="1" r="E16">
+      <c r="E16" s="1" t="n">
         <v>41244</v>
       </c>
-      <c t="s" r="F16">
+      <c r="F16" s="0" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="17">
-      <c t="s" r="A17">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="17">
+      <c r="A17" s="0" t="s">
         <v>49</v>
       </c>
-      <c t="s" r="C17">
+      <c r="C17" s="0" t="s">
         <v>44</v>
       </c>
-      <c s="1" r="D17">
+      <c r="D17" s="1" t="n">
         <v>41215</v>
       </c>
-      <c s="1" r="E17">
+      <c r="E17" s="1" t="n">
         <v>41244</v>
       </c>
-      <c t="s" r="F17">
+      <c r="F17" s="0" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="18">
-      <c t="s" r="A18">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="18">
+      <c r="A18" s="0" t="s">
         <v>51</v>
       </c>
-      <c t="s" r="C18">
+      <c r="C18" s="0" t="s">
         <v>15</v>
       </c>
-      <c s="1" r="D18">
+      <c r="D18" s="1" t="n">
         <v>41230</v>
       </c>
-      <c s="1" r="E18">
+      <c r="E18" s="1" t="n">
         <v>41244</v>
       </c>
-      <c t="s" r="F18">
+      <c r="F18" s="0" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="19">
-      <c t="s" r="A19">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="19">
+      <c r="A19" s="0" t="s">
         <v>53</v>
       </c>
-      <c t="s" r="C19">
+      <c r="C19" s="0" t="s">
         <v>9</v>
       </c>
-      <c s="1" r="D19">
+      <c r="D19" s="1" t="n">
         <v>41215</v>
       </c>
-      <c s="1" r="E19">
+      <c r="E19" s="1" t="n">
         <v>41244</v>
       </c>
-      <c t="s" r="F19">
+      <c r="F19" s="0" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="20">
-      <c t="s" r="A20">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="20">
+      <c r="A20" s="0" t="s">
         <v>55</v>
       </c>
-      <c t="s" r="B20">
+      <c r="B20" s="0" t="s">
         <v>56</v>
       </c>
-      <c t="s" r="C20">
+      <c r="C20" s="0" t="s">
         <v>44</v>
       </c>
-      <c s="1" r="D20">
+      <c r="D20" s="1" t="n">
         <v>41244</v>
       </c>
-      <c s="1" r="E20">
+      <c r="E20" s="1" t="n">
         <v>41310</v>
       </c>
-      <c t="s" r="F20">
+      <c r="F20" s="0" t="s">
         <v>57</v>
       </c>
-      <c t="s" r="G20">
+      <c r="G20" s="0" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="21">
-      <c t="s" r="A21">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="21">
+      <c r="A21" s="0" t="s">
         <v>59</v>
       </c>
-      <c t="s" r="C21">
+      <c r="C21" s="0" t="s">
         <v>41</v>
       </c>
-      <c s="1" r="D21">
+      <c r="D21" s="1" t="n">
         <v>41303</v>
       </c>
-      <c s="1" r="E21">
+      <c r="E21" s="1" t="n">
         <v>41315</v>
       </c>
-      <c t="s" r="F21">
+      <c r="F21" s="0" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="22">
-      <c t="s" r="A22">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="22">
+      <c r="A22" s="0" t="s">
         <v>61</v>
       </c>
-      <c t="s" r="C22">
+      <c r="C22" s="0" t="s">
         <v>28</v>
       </c>
-      <c s="1" r="D22">
+      <c r="D22" s="1" t="n">
         <v>41303</v>
       </c>
-      <c s="1" r="E22">
+      <c r="E22" s="1" t="n">
         <v>41315</v>
       </c>
-      <c t="s" r="F22">
+      <c r="F22" s="0" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="23">
-      <c t="s" r="A23">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="23">
+      <c r="A23" s="0" t="s">
         <v>63</v>
       </c>
-      <c t="s" r="C23">
+      <c r="C23" s="0" t="s">
         <v>9</v>
       </c>
-      <c s="1" r="D23">
+      <c r="D23" s="1" t="n">
         <v>40945</v>
       </c>
-      <c s="1" r="E23">
+      <c r="E23" s="1" t="n">
         <v>40955</v>
       </c>
-      <c t="s" r="F23">
+      <c r="F23" s="0" t="s">
         <v>64</v>
       </c>
-      <c t="s" r="G23">
+      <c r="G23" s="0" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="24">
-      <c t="s" r="A24">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="24">
+      <c r="A24" s="0" t="s">
         <v>66</v>
       </c>
-      <c t="s" r="B24">
+      <c r="B24" s="0" t="s">
         <v>67</v>
       </c>
-      <c t="s" r="C24">
+      <c r="C24" s="0" t="s">
         <v>15</v>
       </c>
-      <c s="1" r="D24">
+      <c r="D24" s="1" t="n">
         <v>40945</v>
       </c>
-      <c s="1" r="E24">
+      <c r="E24" s="1" t="n">
         <v>40955</v>
       </c>
-      <c t="s" r="F24">
+      <c r="F24" s="0" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="25">
-      <c t="s" r="A25">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="25">
+      <c r="A25" s="0" t="s">
         <v>69</v>
       </c>
-      <c t="s" r="B25">
+      <c r="B25" s="0" t="s">
         <v>70</v>
       </c>
-      <c t="s" r="C25">
+      <c r="C25" s="0" t="s">
         <v>23</v>
       </c>
-      <c s="1" r="D25">
+      <c r="D25" s="1" t="n">
         <v>40945</v>
       </c>
-      <c s="1" r="E25">
+      <c r="E25" s="1" t="n">
         <v>40955</v>
       </c>
-      <c t="s" r="F25">
+      <c r="F25" s="0" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="26">
-      <c t="s" r="A26">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="26">
+      <c r="A26" s="0" t="s">
         <v>72</v>
       </c>
-      <c t="s" r="B26">
+      <c r="B26" s="0" t="s">
         <v>73</v>
       </c>
-      <c t="s" r="C26">
+      <c r="C26" s="0" t="s">
         <v>41</v>
       </c>
-      <c s="1" r="D26">
+      <c r="D26" s="1" t="n">
         <v>40949</v>
       </c>
-      <c s="1" r="E26">
+      <c r="E26" s="1" t="n">
         <v>40955</v>
       </c>
-      <c t="s" r="F26">
+      <c r="F26" s="0" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="27">
-      <c t="s" r="A27">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="27">
+      <c r="A27" s="0" t="s">
         <v>75</v>
       </c>
-      <c t="s" r="B27">
+      <c r="B27" s="0" t="s">
         <v>76</v>
       </c>
-      <c t="s" r="C27">
+      <c r="C27" s="0" t="s">
         <v>28</v>
       </c>
-      <c s="1" r="D27">
+      <c r="D27" s="1" t="n">
         <v>40949</v>
       </c>
-      <c s="1" r="E27">
+      <c r="E27" s="1" t="n">
         <v>40955</v>
       </c>
-      <c t="s" r="F27">
+      <c r="F27" s="0" t="s">
         <v>77</v>
       </c>
     </row>
   </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Editted SE_N15_TEST_01 Additional Members
Added myself to the additional Members of ID SE_N15_TEST_01
</commit_message>
<xml_diff>
--- a/n15/docs/Gantt-chart.xlsx
+++ b/n15/docs/Gantt-chart.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="78">
   <si>
     <t>ID</t>
   </si>
@@ -350,19 +350,19 @@
   <dimension ref="A1:G27"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="G13" activeCellId="0" pane="topLeft" sqref="G13"/>
+      <selection activeCell="F17" activeCellId="0" pane="topLeft" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.8117647058824"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="28"/>
-    <col collapsed="false" hidden="false" max="5" min="3" style="0" width="17.2196078431373"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="42.3450980392157"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="37.3254901960784"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="17.2196078431373"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.9176470588235"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="28.1372549019608"/>
+    <col collapsed="false" hidden="false" max="5" min="3" style="0" width="17.3019607843137"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="42.5607843137255"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="37.5176470588235"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="17.3019607843137"/>
   </cols>
   <sheetData>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="1">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="1">
       <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
@@ -385,7 +385,7 @@
         <v>6</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="2">
       <c r="A2" s="0" t="s">
         <v>7</v>
       </c>
@@ -405,7 +405,7 @@
         <v>10</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="3">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="3">
       <c r="A3" s="0" t="s">
         <v>11</v>
       </c>
@@ -422,7 +422,7 @@
         <v>13</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="4">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="4">
       <c r="A4" s="0" t="s">
         <v>14</v>
       </c>
@@ -439,7 +439,7 @@
         <v>16</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="5">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="5">
       <c r="A5" s="0" t="s">
         <v>17</v>
       </c>
@@ -456,7 +456,7 @@
         <v>19</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="6">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="6">
       <c r="A6" s="0" t="s">
         <v>20</v>
       </c>
@@ -473,7 +473,7 @@
         <v>21</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="7">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="7">
       <c r="A7" s="0" t="s">
         <v>22</v>
       </c>
@@ -489,8 +489,11 @@
       <c r="F7" s="0" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="8">
+      <c r="G7" s="0" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="8">
       <c r="A8" s="0" t="s">
         <v>25</v>
       </c>
@@ -513,7 +516,7 @@
         <v>28</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="9">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="9">
       <c r="A9" s="0" t="s">
         <v>29</v>
       </c>
@@ -536,7 +539,7 @@
         <v>28</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="10">
       <c r="A10" s="0" t="s">
         <v>32</v>
       </c>
@@ -556,7 +559,7 @@
         <v>10</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="11">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="11">
       <c r="A11" s="0" t="s">
         <v>34</v>
       </c>
@@ -573,7 +576,7 @@
         <v>35</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="12">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="12">
       <c r="A12" s="0" t="s">
         <v>36</v>
       </c>
@@ -590,7 +593,7 @@
         <v>37</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="13">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="13">
       <c r="A13" s="0" t="s">
         <v>38</v>
       </c>
@@ -607,7 +610,7 @@
         <v>39</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="14">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="14">
       <c r="A14" s="0" t="s">
         <v>40</v>
       </c>
@@ -624,7 +627,7 @@
         <v>42</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="15">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="15">
       <c r="A15" s="0" t="s">
         <v>43</v>
       </c>
@@ -641,7 +644,7 @@
         <v>45</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="16">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="16">
       <c r="A16" s="0" t="s">
         <v>46</v>
       </c>
@@ -661,7 +664,7 @@
         <v>48</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="17">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="17">
       <c r="A17" s="0" t="s">
         <v>49</v>
       </c>
@@ -678,7 +681,7 @@
         <v>50</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="18">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="18">
       <c r="A18" s="0" t="s">
         <v>51</v>
       </c>
@@ -695,7 +698,7 @@
         <v>52</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="19">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="19">
       <c r="A19" s="0" t="s">
         <v>53</v>
       </c>
@@ -712,7 +715,7 @@
         <v>54</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="20">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="20">
       <c r="A20" s="0" t="s">
         <v>55</v>
       </c>
@@ -735,7 +738,7 @@
         <v>58</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="21">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="21">
       <c r="A21" s="0" t="s">
         <v>59</v>
       </c>
@@ -752,7 +755,7 @@
         <v>60</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="22">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="22">
       <c r="A22" s="0" t="s">
         <v>61</v>
       </c>
@@ -769,7 +772,7 @@
         <v>62</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="23">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="23">
       <c r="A23" s="0" t="s">
         <v>63</v>
       </c>
@@ -789,7 +792,7 @@
         <v>65</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="24">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="24">
       <c r="A24" s="0" t="s">
         <v>66</v>
       </c>
@@ -809,7 +812,7 @@
         <v>68</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="25">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="25">
       <c r="A25" s="0" t="s">
         <v>69</v>
       </c>
@@ -829,7 +832,7 @@
         <v>71</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="26">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="26">
       <c r="A26" s="0" t="s">
         <v>72</v>
       </c>
@@ -849,7 +852,7 @@
         <v>74</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="27">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="27">
       <c r="A27" s="0" t="s">
         <v>75</v>
       </c>

</xml_diff>